<commit_message>
Added different popup title for community layers per https://github.com/Innovate-Inc/EnviroAtlas/issues/289
</commit_message>
<xml_diff>
--- a/scripts/EAWAB4JSON.xlsx
+++ b/scripts/EAWAB4JSON.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\EnviroAtlas\FY2017_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\wwwroot\EnviroAtlas\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,10 +22,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALL (TopicInBC)'!$A$1:$X$495</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">BOUNDARY!$A$1:$AC$50</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EA_main!$A$1:$AC$403</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EA_main!$A$1:$AC$402</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PBS!$A$1:$W$90</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -5968,7 +5968,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="28">
     <font>
       <sz val="11"/>
@@ -6747,6 +6747,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -6782,6 +6799,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -32983,9 +33017,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W354"/>
+  <dimension ref="A1:W353"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
+      <selection activeCell="A307" sqref="A307:XFD307"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -48435,16 +48471,13 @@
       <c r="V306" s="2"/>
     </row>
     <row r="307" spans="1:22" ht="15" customHeight="1">
-      <c r="A307" s="2">
-        <v>306</v>
-      </c>
       <c r="B307" s="2"/>
-      <c r="C307" s="53"/>
-      <c r="T307" s="7"/>
       <c r="V307" s="71"/>
     </row>
     <row r="308" spans="1:22" ht="15" customHeight="1">
       <c r="B308" s="2"/>
+      <c r="C308" s="53"/>
+      <c r="T308" s="99"/>
       <c r="V308" s="71"/>
     </row>
     <row r="309" spans="1:22" ht="15" customHeight="1">
@@ -48491,8 +48524,6 @@
     </row>
     <row r="316" spans="1:22" ht="15" customHeight="1">
       <c r="B316" s="2"/>
-      <c r="C316" s="53"/>
-      <c r="T316" s="99"/>
       <c r="V316" s="71"/>
     </row>
     <row r="317" spans="1:22" ht="15" customHeight="1">
@@ -48505,6 +48536,8 @@
     </row>
     <row r="319" spans="1:22" ht="15" customHeight="1">
       <c r="B319" s="2"/>
+      <c r="C319" s="100"/>
+      <c r="T319" s="7"/>
       <c r="V319" s="71"/>
     </row>
     <row r="320" spans="1:22" ht="15" customHeight="1">
@@ -48515,7 +48548,7 @@
     </row>
     <row r="321" spans="2:22" ht="15" customHeight="1">
       <c r="B321" s="2"/>
-      <c r="C321" s="100"/>
+      <c r="C321" s="53"/>
       <c r="T321" s="7"/>
       <c r="V321" s="71"/>
     </row>
@@ -48573,7 +48606,7 @@
       <c r="T330" s="7"/>
       <c r="V330" s="71"/>
     </row>
-    <row r="331" spans="2:22" ht="15" customHeight="1">
+    <row r="331" spans="2:22">
       <c r="B331" s="2"/>
       <c r="C331" s="53"/>
       <c r="T331" s="7"/>
@@ -48587,13 +48620,13 @@
     </row>
     <row r="333" spans="2:22">
       <c r="B333" s="2"/>
-      <c r="C333" s="53"/>
+      <c r="C333" s="101"/>
       <c r="T333" s="7"/>
       <c r="V333" s="71"/>
     </row>
     <row r="334" spans="2:22">
       <c r="B334" s="2"/>
-      <c r="C334" s="101"/>
+      <c r="C334" s="53"/>
       <c r="T334" s="7"/>
       <c r="V334" s="71"/>
     </row>
@@ -48612,7 +48645,7 @@
     <row r="337" spans="2:22">
       <c r="B337" s="2"/>
       <c r="C337" s="53"/>
-      <c r="T337" s="7"/>
+      <c r="T337" s="99"/>
       <c r="V337" s="71"/>
     </row>
     <row r="338" spans="2:22">
@@ -48647,12 +48680,12 @@
     </row>
     <row r="343" spans="2:22">
       <c r="B343" s="2"/>
-      <c r="C343" s="53"/>
-      <c r="T343" s="99"/>
       <c r="V343" s="71"/>
     </row>
     <row r="344" spans="2:22">
       <c r="B344" s="2"/>
+      <c r="C344" s="53"/>
+      <c r="T344" s="99"/>
       <c r="V344" s="71"/>
     </row>
     <row r="345" spans="2:22">
@@ -48670,7 +48703,7 @@
     <row r="347" spans="2:22">
       <c r="B347" s="2"/>
       <c r="C347" s="53"/>
-      <c r="T347" s="99"/>
+      <c r="T347" s="7"/>
       <c r="V347" s="71"/>
     </row>
     <row r="348" spans="2:22">
@@ -48681,7 +48714,7 @@
     </row>
     <row r="349" spans="2:22">
       <c r="B349" s="2"/>
-      <c r="C349" s="53"/>
+      <c r="C349" s="102"/>
       <c r="T349" s="7"/>
       <c r="V349" s="71"/>
     </row>
@@ -48705,15 +48738,9 @@
     </row>
     <row r="353" spans="2:22">
       <c r="B353" s="2"/>
-      <c r="C353" s="102"/>
-      <c r="T353" s="7"/>
+      <c r="C353" s="53"/>
+      <c r="T353" s="99"/>
       <c r="V353" s="71"/>
-    </row>
-    <row r="354" spans="2:22">
-      <c r="B354" s="2"/>
-      <c r="C354" s="53"/>
-      <c r="T354" s="99"/>
-      <c r="V354" s="71"/>
     </row>
   </sheetData>
   <sortState ref="A261:W282">

</xml_diff>

<commit_message>
QA updates to config files and local layer widget.
</commit_message>
<xml_diff>
--- a/scripts/EAWAB4JSON.xlsx
+++ b/scripts/EAWAB4JSON.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\EnviroAtlas\FY2017_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\wwwroot\EnviroAtlas\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,12 +25,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EA_main!$A$1:$X$304</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PBS!$A$1:$W$60</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13454" uniqueCount="2383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13451" uniqueCount="2383">
   <si>
     <t>Layer Name</t>
   </si>
@@ -7703,7 +7703,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8540,6 +8540,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8575,6 +8592,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -40434,9 +40468,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z504"/>
+  <dimension ref="A1:Z501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q448" workbookViewId="0">
+      <selection activeCell="Q479" sqref="A479:XFD481"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -40454,7 +40490,7 @@
     <col min="20" max="20" width="32.5703125" style="2" customWidth="1"/>
     <col min="21" max="21" width="34" style="2" customWidth="1"/>
     <col min="22" max="23" width="18.7109375" style="3" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="73.5703125" style="2" customWidth="1"/>
     <col min="25" max="25" width="18.7109375" style="3" customWidth="1"/>
     <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -60590,7 +60626,10 @@
         <v xml:space="preserve">Recreation, Culture, and Aesthetics - x; </v>
       </c>
     </row>
-    <row r="305" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A305" s="2">
+        <v>304</v>
+      </c>
       <c r="B305" s="2" t="s">
         <v>176</v>
       </c>
@@ -60648,91 +60687,91 @@
         <v xml:space="preserve">Recreation, Culture, and Aesthetics - x; </v>
       </c>
     </row>
-    <row r="306" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z306" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="307" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z307" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="308" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z308" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="309" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z309" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="310" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z310" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="311" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z311" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="312" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z312" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="313" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z313" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="314" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z314" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="315" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z315" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="316" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z316" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="317" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z317" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="318" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z318" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="319" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z319" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="320" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z320" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -61423,23 +61462,26 @@
       </c>
     </row>
     <row r="479" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z479" s="2" t="s">
-        <v>2194</v>
+      <c r="Z479" s="2" t="str">
+        <f t="shared" ref="Z479:Z501" si="9">IF(LEN(TRIM(L479))=0,"",$L$1 &amp; " - " &amp; L479 &amp; "; ") &amp; IF(LEN(TRIM(M479))=0,"",$M$1 &amp; " - " &amp; M479 &amp; "; ") &amp; IF(LEN(TRIM(N479))=0,"",$N$1 &amp; " - " &amp; N479 &amp; "; ") &amp; IF(LEN(TRIM(O479))=0,"",$O$1 &amp; " - " &amp; O479 &amp; "; ") &amp; IF(LEN(TRIM(P479))=0,"",$P$1 &amp; " - " &amp; P479 &amp; "; ") &amp; IF(LEN(TRIM(Q479))=0,"",$Q$1 &amp; " - " &amp; Q479 &amp; "; ") &amp; IF(LEN(TRIM(R479))=0,"",$R$1 &amp; " - " &amp; R479 &amp; "; ")</f>
+        <v/>
       </c>
     </row>
     <row r="480" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z480" s="2" t="s">
-        <v>2194</v>
+      <c r="Z480" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="481" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z481" s="2" t="s">
-        <v>2194</v>
+      <c r="Z481" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="482" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z482" s="2" t="str">
-        <f t="shared" ref="Z482:Z504" si="9">IF(LEN(TRIM(L482))=0,"",$L$1 &amp; " - " &amp; L482 &amp; "; ") &amp; IF(LEN(TRIM(M482))=0,"",$M$1 &amp; " - " &amp; M482 &amp; "; ") &amp; IF(LEN(TRIM(N482))=0,"",$N$1 &amp; " - " &amp; N482 &amp; "; ") &amp; IF(LEN(TRIM(O482))=0,"",$O$1 &amp; " - " &amp; O482 &amp; "; ") &amp; IF(LEN(TRIM(P482))=0,"",$P$1 &amp; " - " &amp; P482 &amp; "; ") &amp; IF(LEN(TRIM(Q482))=0,"",$Q$1 &amp; " - " &amp; Q482 &amp; "; ") &amp; IF(LEN(TRIM(R482))=0,"",$R$1 &amp; " - " &amp; R482 &amp; "; ")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -61553,24 +61595,6 @@
     </row>
     <row r="501" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z501" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-    </row>
-    <row r="502" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z502" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-    </row>
-    <row r="503" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z503" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-    </row>
-    <row r="504" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z504" s="2" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>

</xml_diff>